<commit_message>
edits for manuscript revisions per MOC & GB
</commit_message>
<xml_diff>
--- a/species_table_pct.xlsx
+++ b/species_table_pct.xlsx
@@ -1,29 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20387"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20392"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slane84\OneDrive - The University Of British Columbia\Documents\Dissertation\CommunityStability\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:40009_{AB9EA1FD-C9F8-4EF7-9C98-EC9C7CE3415D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{8FF34540-4FC7-4C1D-880E-51A76D1BD39A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{139848B6-F144-451A-86A7-152D89BDF0FF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6350" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="species_table_pct" sheetId="1" r:id="rId1"/>
+    <sheet name="table" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">species_table_pct!$A$1:$G$163</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">table!$A$1:$G$163</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="84">
   <si>
     <t>Assemblage</t>
   </si>
@@ -260,6 +262,21 @@
   </si>
   <si>
     <t>Symphyotrichum subspicatum</t>
+  </si>
+  <si>
+    <t>&lt; 0.1</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>lost</t>
+  </si>
+  <si>
+    <t>Overall Change (1979-2019)</t>
+  </si>
+  <si>
+    <t>gained</t>
   </si>
 </sst>
 </file>
@@ -594,7 +611,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -881,6 +898,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -926,7 +978,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -990,6 +1042,61 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1358,8 +1465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G163"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1395,10 +1502,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="46" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="13" t="s">
@@ -1419,8 +1526,8 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="28"/>
-      <c r="B3" s="28"/>
+      <c r="A3" s="47"/>
+      <c r="B3" s="47"/>
       <c r="C3" s="7" t="s">
         <v>36</v>
       </c>
@@ -1439,8 +1546,8 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="28"/>
-      <c r="B4" s="28"/>
+      <c r="A4" s="47"/>
+      <c r="B4" s="47"/>
       <c r="C4" s="13" t="s">
         <v>4</v>
       </c>
@@ -1459,8 +1566,8 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="28"/>
-      <c r="B5" s="28"/>
+      <c r="A5" s="47"/>
+      <c r="B5" s="47"/>
       <c r="C5" s="7" t="s">
         <v>31</v>
       </c>
@@ -1479,8 +1586,8 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="28"/>
-      <c r="B6" s="28"/>
+      <c r="A6" s="47"/>
+      <c r="B6" s="47"/>
       <c r="C6" s="13" t="s">
         <v>76</v>
       </c>
@@ -1499,8 +1606,8 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="28"/>
-      <c r="B7" s="28"/>
+      <c r="A7" s="47"/>
+      <c r="B7" s="47"/>
       <c r="C7" s="7" t="s">
         <v>33</v>
       </c>
@@ -1519,8 +1626,8 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="28"/>
-      <c r="B8" s="28"/>
+      <c r="A8" s="47"/>
+      <c r="B8" s="47"/>
       <c r="C8" s="13" t="s">
         <v>23</v>
       </c>
@@ -1538,8 +1645,8 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="28"/>
-      <c r="B9" s="28"/>
+      <c r="A9" s="47"/>
+      <c r="B9" s="47"/>
       <c r="C9" s="16" t="s">
         <v>77</v>
       </c>
@@ -1557,8 +1664,8 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="28"/>
-      <c r="B10" s="28"/>
+      <c r="A10" s="47"/>
+      <c r="B10" s="47"/>
       <c r="C10" s="13" t="s">
         <v>38</v>
       </c>
@@ -1576,8 +1683,8 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="28"/>
-      <c r="B11" s="29"/>
+      <c r="A11" s="47"/>
+      <c r="B11" s="48"/>
       <c r="C11" s="10" t="s">
         <v>18</v>
       </c>
@@ -1595,8 +1702,8 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="28"/>
-      <c r="B12" s="27" t="s">
+      <c r="A12" s="47"/>
+      <c r="B12" s="46" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="4" t="s">
@@ -1617,8 +1724,8 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="28"/>
-      <c r="B13" s="28"/>
+      <c r="A13" s="47"/>
+      <c r="B13" s="47"/>
       <c r="C13" s="13" t="s">
         <v>6</v>
       </c>
@@ -1632,13 +1739,13 @@
         <v>0</v>
       </c>
       <c r="G13" s="15">
-        <f t="shared" ref="G12:G35" si="1">((D13-F13)/D13)*-100</f>
+        <f t="shared" ref="G13:G35" si="1">((D13-F13)/D13)*-100</f>
         <v>-100</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="28"/>
-      <c r="B14" s="28"/>
+      <c r="A14" s="47"/>
+      <c r="B14" s="47"/>
       <c r="C14" s="7" t="s">
         <v>12</v>
       </c>
@@ -1657,8 +1764,8 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="28"/>
-      <c r="B15" s="28"/>
+      <c r="A15" s="47"/>
+      <c r="B15" s="47"/>
       <c r="C15" s="13" t="s">
         <v>15</v>
       </c>
@@ -1677,8 +1784,8 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="28"/>
-      <c r="B16" s="28"/>
+      <c r="A16" s="47"/>
+      <c r="B16" s="47"/>
       <c r="C16" s="7" t="s">
         <v>28</v>
       </c>
@@ -1697,8 +1804,8 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="28"/>
-      <c r="B17" s="28"/>
+      <c r="A17" s="47"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="13" t="s">
         <v>29</v>
       </c>
@@ -1717,8 +1824,8 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="28"/>
-      <c r="B18" s="28"/>
+      <c r="A18" s="47"/>
+      <c r="B18" s="47"/>
       <c r="C18" s="7" t="s">
         <v>37</v>
       </c>
@@ -1737,8 +1844,8 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" s="28"/>
-      <c r="B19" s="28"/>
+      <c r="A19" s="47"/>
+      <c r="B19" s="47"/>
       <c r="C19" s="13" t="s">
         <v>43</v>
       </c>
@@ -1757,8 +1864,8 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="28"/>
-      <c r="B20" s="28"/>
+      <c r="A20" s="47"/>
+      <c r="B20" s="47"/>
       <c r="C20" s="7" t="s">
         <v>51</v>
       </c>
@@ -1777,8 +1884,8 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" s="28"/>
-      <c r="B21" s="28"/>
+      <c r="A21" s="47"/>
+      <c r="B21" s="47"/>
       <c r="C21" s="13" t="s">
         <v>11</v>
       </c>
@@ -1797,8 +1904,8 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" s="28"/>
-      <c r="B22" s="28"/>
+      <c r="A22" s="47"/>
+      <c r="B22" s="47"/>
       <c r="C22" s="7" t="s">
         <v>9</v>
       </c>
@@ -1817,8 +1924,8 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="28"/>
-      <c r="B23" s="28"/>
+      <c r="A23" s="47"/>
+      <c r="B23" s="47"/>
       <c r="C23" s="13" t="s">
         <v>52</v>
       </c>
@@ -1837,8 +1944,8 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="28"/>
-      <c r="B24" s="28"/>
+      <c r="A24" s="47"/>
+      <c r="B24" s="47"/>
       <c r="C24" s="7" t="s">
         <v>49</v>
       </c>
@@ -1857,8 +1964,8 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" s="28"/>
-      <c r="B25" s="28"/>
+      <c r="A25" s="47"/>
+      <c r="B25" s="47"/>
       <c r="C25" s="13" t="s">
         <v>13</v>
       </c>
@@ -1877,8 +1984,8 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" s="28"/>
-      <c r="B26" s="28"/>
+      <c r="A26" s="47"/>
+      <c r="B26" s="47"/>
       <c r="C26" s="7" t="s">
         <v>78</v>
       </c>
@@ -1897,8 +2004,8 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" s="28"/>
-      <c r="B27" s="28"/>
+      <c r="A27" s="47"/>
+      <c r="B27" s="47"/>
       <c r="C27" s="13" t="s">
         <v>26</v>
       </c>
@@ -1917,8 +2024,8 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" s="28"/>
-      <c r="B28" s="28"/>
+      <c r="A28" s="47"/>
+      <c r="B28" s="47"/>
       <c r="C28" s="7" t="s">
         <v>39</v>
       </c>
@@ -1937,8 +2044,8 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A29" s="28"/>
-      <c r="B29" s="28"/>
+      <c r="A29" s="47"/>
+      <c r="B29" s="47"/>
       <c r="C29" s="13" t="s">
         <v>35</v>
       </c>
@@ -1957,8 +2064,8 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A30" s="28"/>
-      <c r="B30" s="28"/>
+      <c r="A30" s="47"/>
+      <c r="B30" s="47"/>
       <c r="C30" s="7" t="s">
         <v>32</v>
       </c>
@@ -1977,8 +2084,8 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A31" s="28"/>
-      <c r="B31" s="28"/>
+      <c r="A31" s="47"/>
+      <c r="B31" s="47"/>
       <c r="C31" s="13" t="s">
         <v>25</v>
       </c>
@@ -1997,8 +2104,8 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A32" s="28"/>
-      <c r="B32" s="28"/>
+      <c r="A32" s="47"/>
+      <c r="B32" s="47"/>
       <c r="C32" s="7" t="s">
         <v>50</v>
       </c>
@@ -2017,8 +2124,8 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A33" s="28"/>
-      <c r="B33" s="28"/>
+      <c r="A33" s="47"/>
+      <c r="B33" s="47"/>
       <c r="C33" s="13" t="s">
         <v>10</v>
       </c>
@@ -2037,8 +2144,8 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A34" s="28"/>
-      <c r="B34" s="28"/>
+      <c r="A34" s="47"/>
+      <c r="B34" s="47"/>
       <c r="C34" s="7" t="s">
         <v>45</v>
       </c>
@@ -2057,8 +2164,8 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A35" s="28"/>
-      <c r="B35" s="28"/>
+      <c r="A35" s="47"/>
+      <c r="B35" s="47"/>
       <c r="C35" s="13" t="s">
         <v>42</v>
       </c>
@@ -2077,8 +2184,8 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A36" s="28"/>
-      <c r="B36" s="28"/>
+      <c r="A36" s="47"/>
+      <c r="B36" s="47"/>
       <c r="C36" s="7" t="s">
         <v>14</v>
       </c>
@@ -2096,8 +2203,8 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A37" s="28"/>
-      <c r="B37" s="28"/>
+      <c r="A37" s="47"/>
+      <c r="B37" s="47"/>
       <c r="C37" s="13" t="s">
         <v>20</v>
       </c>
@@ -2115,8 +2222,8 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A38" s="28"/>
-      <c r="B38" s="28"/>
+      <c r="A38" s="47"/>
+      <c r="B38" s="47"/>
       <c r="C38" s="7" t="s">
         <v>21</v>
       </c>
@@ -2134,8 +2241,8 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A39" s="28"/>
-      <c r="B39" s="28"/>
+      <c r="A39" s="47"/>
+      <c r="B39" s="47"/>
       <c r="C39" s="13" t="s">
         <v>22</v>
       </c>
@@ -2153,8 +2260,8 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A40" s="28"/>
-      <c r="B40" s="28"/>
+      <c r="A40" s="47"/>
+      <c r="B40" s="47"/>
       <c r="C40" s="7" t="s">
         <v>24</v>
       </c>
@@ -2172,8 +2279,8 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A41" s="28"/>
-      <c r="B41" s="28"/>
+      <c r="A41" s="47"/>
+      <c r="B41" s="47"/>
       <c r="C41" s="13" t="s">
         <v>27</v>
       </c>
@@ -2191,8 +2298,8 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A42" s="28"/>
-      <c r="B42" s="28"/>
+      <c r="A42" s="47"/>
+      <c r="B42" s="47"/>
       <c r="C42" s="7" t="s">
         <v>30</v>
       </c>
@@ -2210,8 +2317,8 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A43" s="28"/>
-      <c r="B43" s="28"/>
+      <c r="A43" s="47"/>
+      <c r="B43" s="47"/>
       <c r="C43" s="13" t="s">
         <v>47</v>
       </c>
@@ -2229,8 +2336,8 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A44" s="28"/>
-      <c r="B44" s="28"/>
+      <c r="A44" s="47"/>
+      <c r="B44" s="47"/>
       <c r="C44" s="7" t="s">
         <v>48</v>
       </c>
@@ -2248,8 +2355,8 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A45" s="28"/>
-      <c r="B45" s="28"/>
+      <c r="A45" s="47"/>
+      <c r="B45" s="47"/>
       <c r="C45" s="13" t="s">
         <v>53</v>
       </c>
@@ -2267,8 +2374,8 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A46" s="28"/>
-      <c r="B46" s="28"/>
+      <c r="A46" s="47"/>
+      <c r="B46" s="47"/>
       <c r="C46" s="7" t="s">
         <v>16</v>
       </c>
@@ -2286,8 +2393,8 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A47" s="28"/>
-      <c r="B47" s="28"/>
+      <c r="A47" s="47"/>
+      <c r="B47" s="47"/>
       <c r="C47" s="13" t="s">
         <v>17</v>
       </c>
@@ -2305,8 +2412,8 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A48" s="28"/>
-      <c r="B48" s="28"/>
+      <c r="A48" s="47"/>
+      <c r="B48" s="47"/>
       <c r="C48" s="7" t="s">
         <v>19</v>
       </c>
@@ -2324,8 +2431,8 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A49" s="28"/>
-      <c r="B49" s="28"/>
+      <c r="A49" s="47"/>
+      <c r="B49" s="47"/>
       <c r="C49" s="13" t="s">
         <v>41</v>
       </c>
@@ -2343,8 +2450,8 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A50" s="28"/>
-      <c r="B50" s="28"/>
+      <c r="A50" s="47"/>
+      <c r="B50" s="47"/>
       <c r="C50" s="13" t="s">
         <v>40</v>
       </c>
@@ -2362,8 +2469,8 @@
       </c>
     </row>
     <row r="51" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="29"/>
-      <c r="B51" s="29"/>
+      <c r="A51" s="48"/>
+      <c r="B51" s="48"/>
       <c r="C51" s="10" t="s">
         <v>46</v>
       </c>
@@ -2413,7 +2520,7 @@
       </c>
     </row>
     <row r="54" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A54" s="27" t="s">
+      <c r="A54" s="46" t="s">
         <v>54</v>
       </c>
       <c r="B54" s="23" t="s">
@@ -2437,8 +2544,8 @@
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A55" s="28"/>
-      <c r="B55" s="27" t="s">
+      <c r="A55" s="47"/>
+      <c r="B55" s="46" t="s">
         <v>5</v>
       </c>
       <c r="C55" s="4" t="s">
@@ -2459,8 +2566,8 @@
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A56" s="28"/>
-      <c r="B56" s="28"/>
+      <c r="A56" s="47"/>
+      <c r="B56" s="47"/>
       <c r="C56" s="13" t="s">
         <v>36</v>
       </c>
@@ -2479,8 +2586,8 @@
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A57" s="28"/>
-      <c r="B57" s="28"/>
+      <c r="A57" s="47"/>
+      <c r="B57" s="47"/>
       <c r="C57" s="7" t="s">
         <v>34</v>
       </c>
@@ -2499,8 +2606,8 @@
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A58" s="28"/>
-      <c r="B58" s="28"/>
+      <c r="A58" s="47"/>
+      <c r="B58" s="47"/>
       <c r="C58" s="13" t="s">
         <v>18</v>
       </c>
@@ -2519,8 +2626,8 @@
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A59" s="28"/>
-      <c r="B59" s="28"/>
+      <c r="A59" s="47"/>
+      <c r="B59" s="47"/>
       <c r="C59" s="7" t="s">
         <v>31</v>
       </c>
@@ -2539,8 +2646,8 @@
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A60" s="28"/>
-      <c r="B60" s="28"/>
+      <c r="A60" s="47"/>
+      <c r="B60" s="47"/>
       <c r="C60" s="13" t="s">
         <v>4</v>
       </c>
@@ -2559,8 +2666,8 @@
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A61" s="28"/>
-      <c r="B61" s="28"/>
+      <c r="A61" s="47"/>
+      <c r="B61" s="47"/>
       <c r="C61" s="7" t="s">
         <v>38</v>
       </c>
@@ -2579,8 +2686,8 @@
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A62" s="28"/>
-      <c r="B62" s="28"/>
+      <c r="A62" s="47"/>
+      <c r="B62" s="47"/>
       <c r="C62" s="13" t="s">
         <v>57</v>
       </c>
@@ -2598,8 +2705,8 @@
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A63" s="28"/>
-      <c r="B63" s="28"/>
+      <c r="A63" s="47"/>
+      <c r="B63" s="47"/>
       <c r="C63" s="13" t="s">
         <v>23</v>
       </c>
@@ -2617,8 +2724,8 @@
       </c>
     </row>
     <row r="64" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A64" s="28"/>
-      <c r="B64" s="29"/>
+      <c r="A64" s="47"/>
+      <c r="B64" s="48"/>
       <c r="C64" s="10" t="s">
         <v>77</v>
       </c>
@@ -2636,8 +2743,8 @@
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A65" s="28"/>
-      <c r="B65" s="27" t="s">
+      <c r="A65" s="47"/>
+      <c r="B65" s="46" t="s">
         <v>7</v>
       </c>
       <c r="C65" s="4" t="s">
@@ -2658,8 +2765,8 @@
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A66" s="28"/>
-      <c r="B66" s="28"/>
+      <c r="A66" s="47"/>
+      <c r="B66" s="47"/>
       <c r="C66" s="13" t="s">
         <v>6</v>
       </c>
@@ -2678,8 +2785,8 @@
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A67" s="28"/>
-      <c r="B67" s="28"/>
+      <c r="A67" s="47"/>
+      <c r="B67" s="47"/>
       <c r="C67" s="7" t="s">
         <v>9</v>
       </c>
@@ -2698,8 +2805,8 @@
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A68" s="28"/>
-      <c r="B68" s="28"/>
+      <c r="A68" s="47"/>
+      <c r="B68" s="47"/>
       <c r="C68" s="13" t="s">
         <v>12</v>
       </c>
@@ -2718,8 +2825,8 @@
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A69" s="28"/>
-      <c r="B69" s="28"/>
+      <c r="A69" s="47"/>
+      <c r="B69" s="47"/>
       <c r="C69" s="7" t="s">
         <v>58</v>
       </c>
@@ -2738,8 +2845,8 @@
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A70" s="28"/>
-      <c r="B70" s="28"/>
+      <c r="A70" s="47"/>
+      <c r="B70" s="47"/>
       <c r="C70" s="13" t="s">
         <v>13</v>
       </c>
@@ -2758,8 +2865,8 @@
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A71" s="28"/>
-      <c r="B71" s="28"/>
+      <c r="A71" s="47"/>
+      <c r="B71" s="47"/>
       <c r="C71" s="7" t="s">
         <v>16</v>
       </c>
@@ -2778,8 +2885,8 @@
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A72" s="28"/>
-      <c r="B72" s="28"/>
+      <c r="A72" s="47"/>
+      <c r="B72" s="47"/>
       <c r="C72" s="13" t="s">
         <v>20</v>
       </c>
@@ -2798,8 +2905,8 @@
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A73" s="28"/>
-      <c r="B73" s="28"/>
+      <c r="A73" s="47"/>
+      <c r="B73" s="47"/>
       <c r="C73" s="7" t="s">
         <v>62</v>
       </c>
@@ -2818,8 +2925,8 @@
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A74" s="28"/>
-      <c r="B74" s="28"/>
+      <c r="A74" s="47"/>
+      <c r="B74" s="47"/>
       <c r="C74" s="13" t="s">
         <v>25</v>
       </c>
@@ -2838,8 +2945,8 @@
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A75" s="28"/>
-      <c r="B75" s="28"/>
+      <c r="A75" s="47"/>
+      <c r="B75" s="47"/>
       <c r="C75" s="7" t="s">
         <v>28</v>
       </c>
@@ -2858,8 +2965,8 @@
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A76" s="28"/>
-      <c r="B76" s="28"/>
+      <c r="A76" s="47"/>
+      <c r="B76" s="47"/>
       <c r="C76" s="13" t="s">
         <v>29</v>
       </c>
@@ -2878,8 +2985,8 @@
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A77" s="28"/>
-      <c r="B77" s="28"/>
+      <c r="A77" s="47"/>
+      <c r="B77" s="47"/>
       <c r="C77" s="7" t="s">
         <v>64</v>
       </c>
@@ -2898,8 +3005,8 @@
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A78" s="28"/>
-      <c r="B78" s="28"/>
+      <c r="A78" s="47"/>
+      <c r="B78" s="47"/>
       <c r="C78" s="13" t="s">
         <v>37</v>
       </c>
@@ -2918,8 +3025,8 @@
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A79" s="28"/>
-      <c r="B79" s="28"/>
+      <c r="A79" s="47"/>
+      <c r="B79" s="47"/>
       <c r="C79" s="7" t="s">
         <v>39</v>
       </c>
@@ -2938,8 +3045,8 @@
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A80" s="28"/>
-      <c r="B80" s="28"/>
+      <c r="A80" s="47"/>
+      <c r="B80" s="47"/>
       <c r="C80" s="13" t="s">
         <v>41</v>
       </c>
@@ -2958,8 +3065,8 @@
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A81" s="28"/>
-      <c r="B81" s="28"/>
+      <c r="A81" s="47"/>
+      <c r="B81" s="47"/>
       <c r="C81" s="7" t="s">
         <v>43</v>
       </c>
@@ -2978,8 +3085,8 @@
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A82" s="28"/>
-      <c r="B82" s="28"/>
+      <c r="A82" s="47"/>
+      <c r="B82" s="47"/>
       <c r="C82" s="13" t="s">
         <v>66</v>
       </c>
@@ -2998,8 +3105,8 @@
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A83" s="28"/>
-      <c r="B83" s="28"/>
+      <c r="A83" s="47"/>
+      <c r="B83" s="47"/>
       <c r="C83" s="7" t="s">
         <v>46</v>
       </c>
@@ -3018,8 +3125,8 @@
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A84" s="28"/>
-      <c r="B84" s="28"/>
+      <c r="A84" s="47"/>
+      <c r="B84" s="47"/>
       <c r="C84" s="13" t="s">
         <v>67</v>
       </c>
@@ -3038,8 +3145,8 @@
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A85" s="28"/>
-      <c r="B85" s="28"/>
+      <c r="A85" s="47"/>
+      <c r="B85" s="47"/>
       <c r="C85" s="7" t="s">
         <v>51</v>
       </c>
@@ -3058,8 +3165,8 @@
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A86" s="28"/>
-      <c r="B86" s="28"/>
+      <c r="A86" s="47"/>
+      <c r="B86" s="47"/>
       <c r="C86" s="13" t="s">
         <v>78</v>
       </c>
@@ -3078,8 +3185,8 @@
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A87" s="28"/>
-      <c r="B87" s="28"/>
+      <c r="A87" s="47"/>
+      <c r="B87" s="47"/>
       <c r="C87" s="7" t="s">
         <v>52</v>
       </c>
@@ -3098,8 +3205,8 @@
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A88" s="28"/>
-      <c r="B88" s="28"/>
+      <c r="A88" s="47"/>
+      <c r="B88" s="47"/>
       <c r="C88" s="13" t="s">
         <v>35</v>
       </c>
@@ -3118,8 +3225,8 @@
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A89" s="28"/>
-      <c r="B89" s="28"/>
+      <c r="A89" s="47"/>
+      <c r="B89" s="47"/>
       <c r="C89" s="7" t="s">
         <v>11</v>
       </c>
@@ -3138,8 +3245,8 @@
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A90" s="28"/>
-      <c r="B90" s="28"/>
+      <c r="A90" s="47"/>
+      <c r="B90" s="47"/>
       <c r="C90" s="13" t="s">
         <v>47</v>
       </c>
@@ -3158,8 +3265,8 @@
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A91" s="28"/>
-      <c r="B91" s="28"/>
+      <c r="A91" s="47"/>
+      <c r="B91" s="47"/>
       <c r="C91" s="7" t="s">
         <v>10</v>
       </c>
@@ -3178,8 +3285,8 @@
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A92" s="28"/>
-      <c r="B92" s="28"/>
+      <c r="A92" s="47"/>
+      <c r="B92" s="47"/>
       <c r="C92" s="13" t="s">
         <v>42</v>
       </c>
@@ -3198,8 +3305,8 @@
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A93" s="28"/>
-      <c r="B93" s="28"/>
+      <c r="A93" s="47"/>
+      <c r="B93" s="47"/>
       <c r="C93" s="7" t="s">
         <v>50</v>
       </c>
@@ -3218,8 +3325,8 @@
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A94" s="28"/>
-      <c r="B94" s="28"/>
+      <c r="A94" s="47"/>
+      <c r="B94" s="47"/>
       <c r="C94" s="13" t="s">
         <v>32</v>
       </c>
@@ -3238,8 +3345,8 @@
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A95" s="28"/>
-      <c r="B95" s="28"/>
+      <c r="A95" s="47"/>
+      <c r="B95" s="47"/>
       <c r="C95" s="7" t="s">
         <v>53</v>
       </c>
@@ -3258,8 +3365,8 @@
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A96" s="28"/>
-      <c r="B96" s="28"/>
+      <c r="A96" s="47"/>
+      <c r="B96" s="47"/>
       <c r="C96" s="13" t="s">
         <v>61</v>
       </c>
@@ -3278,8 +3385,8 @@
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A97" s="28"/>
-      <c r="B97" s="28"/>
+      <c r="A97" s="47"/>
+      <c r="B97" s="47"/>
       <c r="C97" s="7" t="s">
         <v>15</v>
       </c>
@@ -3298,8 +3405,8 @@
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A98" s="28"/>
-      <c r="B98" s="28"/>
+      <c r="A98" s="47"/>
+      <c r="B98" s="47"/>
       <c r="C98" s="13" t="s">
         <v>49</v>
       </c>
@@ -3318,8 +3425,8 @@
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A99" s="28"/>
-      <c r="B99" s="28"/>
+      <c r="A99" s="47"/>
+      <c r="B99" s="47"/>
       <c r="C99" s="7" t="s">
         <v>27</v>
       </c>
@@ -3338,8 +3445,8 @@
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A100" s="28"/>
-      <c r="B100" s="28"/>
+      <c r="A100" s="47"/>
+      <c r="B100" s="47"/>
       <c r="C100" s="13" t="s">
         <v>45</v>
       </c>
@@ -3358,8 +3465,8 @@
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A101" s="28"/>
-      <c r="B101" s="28"/>
+      <c r="A101" s="47"/>
+      <c r="B101" s="47"/>
       <c r="C101" s="7" t="s">
         <v>22</v>
       </c>
@@ -3378,8 +3485,8 @@
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A102" s="28"/>
-      <c r="B102" s="28"/>
+      <c r="A102" s="47"/>
+      <c r="B102" s="47"/>
       <c r="C102" s="13" t="s">
         <v>14</v>
       </c>
@@ -3397,8 +3504,8 @@
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A103" s="28"/>
-      <c r="B103" s="28"/>
+      <c r="A103" s="47"/>
+      <c r="B103" s="47"/>
       <c r="C103" s="7" t="s">
         <v>63</v>
       </c>
@@ -3416,8 +3523,8 @@
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A104" s="28"/>
-      <c r="B104" s="28"/>
+      <c r="A104" s="47"/>
+      <c r="B104" s="47"/>
       <c r="C104" s="13" t="s">
         <v>30</v>
       </c>
@@ -3435,8 +3542,8 @@
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A105" s="28"/>
-      <c r="B105" s="28"/>
+      <c r="A105" s="47"/>
+      <c r="B105" s="47"/>
       <c r="C105" s="7" t="s">
         <v>65</v>
       </c>
@@ -3454,8 +3561,8 @@
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A106" s="28"/>
-      <c r="B106" s="28"/>
+      <c r="A106" s="47"/>
+      <c r="B106" s="47"/>
       <c r="C106" s="13" t="s">
         <v>48</v>
       </c>
@@ -3473,8 +3580,8 @@
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A107" s="28"/>
-      <c r="B107" s="28"/>
+      <c r="A107" s="47"/>
+      <c r="B107" s="47"/>
       <c r="C107" s="7" t="s">
         <v>55</v>
       </c>
@@ -3492,8 +3599,8 @@
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A108" s="28"/>
-      <c r="B108" s="28"/>
+      <c r="A108" s="47"/>
+      <c r="B108" s="47"/>
       <c r="C108" s="13" t="s">
         <v>56</v>
       </c>
@@ -3511,8 +3618,8 @@
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A109" s="28"/>
-      <c r="B109" s="28"/>
+      <c r="A109" s="47"/>
+      <c r="B109" s="47"/>
       <c r="C109" s="7" t="s">
         <v>19</v>
       </c>
@@ -3530,8 +3637,8 @@
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A110" s="28"/>
-      <c r="B110" s="28"/>
+      <c r="A110" s="47"/>
+      <c r="B110" s="47"/>
       <c r="C110" s="13" t="s">
         <v>26</v>
       </c>
@@ -3549,8 +3656,8 @@
       </c>
     </row>
     <row r="111" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A111" s="29"/>
-      <c r="B111" s="29"/>
+      <c r="A111" s="48"/>
+      <c r="B111" s="48"/>
       <c r="C111" s="10" t="s">
         <v>68</v>
       </c>
@@ -3600,7 +3707,7 @@
       </c>
     </row>
     <row r="114" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A114" s="27" t="s">
+      <c r="A114" s="46" t="s">
         <v>69</v>
       </c>
       <c r="B114" s="23" t="s">
@@ -3623,8 +3730,8 @@
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A115" s="28"/>
-      <c r="B115" s="27" t="s">
+      <c r="A115" s="47"/>
+      <c r="B115" s="46" t="s">
         <v>5</v>
       </c>
       <c r="C115" s="4" t="s">
@@ -3645,8 +3752,8 @@
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A116" s="28"/>
-      <c r="B116" s="28"/>
+      <c r="A116" s="47"/>
+      <c r="B116" s="47"/>
       <c r="C116" s="13" t="s">
         <v>34</v>
       </c>
@@ -3665,8 +3772,8 @@
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A117" s="28"/>
-      <c r="B117" s="28"/>
+      <c r="A117" s="47"/>
+      <c r="B117" s="47"/>
       <c r="C117" s="7" t="s">
         <v>4</v>
       </c>
@@ -3685,8 +3792,8 @@
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A118" s="28"/>
-      <c r="B118" s="28"/>
+      <c r="A118" s="47"/>
+      <c r="B118" s="47"/>
       <c r="C118" s="13" t="s">
         <v>31</v>
       </c>
@@ -3705,8 +3812,8 @@
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A119" s="28"/>
-      <c r="B119" s="28"/>
+      <c r="A119" s="47"/>
+      <c r="B119" s="47"/>
       <c r="C119" s="7" t="s">
         <v>18</v>
       </c>
@@ -3725,8 +3832,8 @@
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A120" s="28"/>
-      <c r="B120" s="28"/>
+      <c r="A120" s="47"/>
+      <c r="B120" s="47"/>
       <c r="C120" s="13" t="s">
         <v>23</v>
       </c>
@@ -3744,8 +3851,8 @@
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A121" s="28"/>
-      <c r="B121" s="28"/>
+      <c r="A121" s="47"/>
+      <c r="B121" s="47"/>
       <c r="C121" s="7" t="s">
         <v>77</v>
       </c>
@@ -3763,8 +3870,8 @@
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A122" s="28"/>
-      <c r="B122" s="28"/>
+      <c r="A122" s="47"/>
+      <c r="B122" s="47"/>
       <c r="C122" s="13" t="s">
         <v>33</v>
       </c>
@@ -3782,8 +3889,8 @@
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A123" s="28"/>
-      <c r="B123" s="28"/>
+      <c r="A123" s="47"/>
+      <c r="B123" s="47"/>
       <c r="C123" s="13" t="s">
         <v>38</v>
       </c>
@@ -3801,8 +3908,8 @@
       </c>
     </row>
     <row r="124" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A124" s="28"/>
-      <c r="B124" s="29"/>
+      <c r="A124" s="47"/>
+      <c r="B124" s="48"/>
       <c r="C124" s="10" t="s">
         <v>57</v>
       </c>
@@ -3820,8 +3927,8 @@
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A125" s="28"/>
-      <c r="B125" s="27" t="s">
+      <c r="A125" s="47"/>
+      <c r="B125" s="46" t="s">
         <v>7</v>
       </c>
       <c r="C125" s="4" t="s">
@@ -3842,8 +3949,8 @@
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A126" s="28"/>
-      <c r="B126" s="28"/>
+      <c r="A126" s="47"/>
+      <c r="B126" s="47"/>
       <c r="C126" s="13" t="s">
         <v>12</v>
       </c>
@@ -3862,8 +3969,8 @@
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A127" s="28"/>
-      <c r="B127" s="28"/>
+      <c r="A127" s="47"/>
+      <c r="B127" s="47"/>
       <c r="C127" s="7" t="s">
         <v>28</v>
       </c>
@@ -3882,8 +3989,8 @@
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A128" s="28"/>
-      <c r="B128" s="28"/>
+      <c r="A128" s="47"/>
+      <c r="B128" s="47"/>
       <c r="C128" s="13" t="s">
         <v>29</v>
       </c>
@@ -3902,8 +4009,8 @@
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A129" s="28"/>
-      <c r="B129" s="28"/>
+      <c r="A129" s="47"/>
+      <c r="B129" s="47"/>
       <c r="C129" s="7" t="s">
         <v>64</v>
       </c>
@@ -3922,8 +4029,8 @@
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A130" s="28"/>
-      <c r="B130" s="28"/>
+      <c r="A130" s="47"/>
+      <c r="B130" s="47"/>
       <c r="C130" s="13" t="s">
         <v>37</v>
       </c>
@@ -3942,8 +4049,8 @@
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A131" s="28"/>
-      <c r="B131" s="28"/>
+      <c r="A131" s="47"/>
+      <c r="B131" s="47"/>
       <c r="C131" s="7" t="s">
         <v>39</v>
       </c>
@@ -3962,8 +4069,8 @@
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A132" s="28"/>
-      <c r="B132" s="28"/>
+      <c r="A132" s="47"/>
+      <c r="B132" s="47"/>
       <c r="C132" s="13" t="s">
         <v>41</v>
       </c>
@@ -3982,8 +4089,8 @@
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A133" s="28"/>
-      <c r="B133" s="28"/>
+      <c r="A133" s="47"/>
+      <c r="B133" s="47"/>
       <c r="C133" s="7" t="s">
         <v>71</v>
       </c>
@@ -4002,8 +4109,8 @@
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A134" s="28"/>
-      <c r="B134" s="28"/>
+      <c r="A134" s="47"/>
+      <c r="B134" s="47"/>
       <c r="C134" s="13" t="s">
         <v>51</v>
       </c>
@@ -4022,8 +4129,8 @@
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A135" s="28"/>
-      <c r="B135" s="28"/>
+      <c r="A135" s="47"/>
+      <c r="B135" s="47"/>
       <c r="C135" s="7" t="s">
         <v>11</v>
       </c>
@@ -4042,8 +4149,8 @@
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A136" s="28"/>
-      <c r="B136" s="28"/>
+      <c r="A136" s="47"/>
+      <c r="B136" s="47"/>
       <c r="C136" s="13" t="s">
         <v>15</v>
       </c>
@@ -4062,8 +4169,8 @@
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A137" s="28"/>
-      <c r="B137" s="28"/>
+      <c r="A137" s="47"/>
+      <c r="B137" s="47"/>
       <c r="C137" s="7" t="s">
         <v>49</v>
       </c>
@@ -4082,8 +4189,8 @@
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A138" s="28"/>
-      <c r="B138" s="28"/>
+      <c r="A138" s="47"/>
+      <c r="B138" s="47"/>
       <c r="C138" s="13" t="s">
         <v>52</v>
       </c>
@@ -4102,8 +4209,8 @@
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A139" s="28"/>
-      <c r="B139" s="28"/>
+      <c r="A139" s="47"/>
+      <c r="B139" s="47"/>
       <c r="C139" s="7" t="s">
         <v>46</v>
       </c>
@@ -4122,8 +4229,8 @@
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A140" s="28"/>
-      <c r="B140" s="28"/>
+      <c r="A140" s="47"/>
+      <c r="B140" s="47"/>
       <c r="C140" s="13" t="s">
         <v>9</v>
       </c>
@@ -4142,8 +4249,8 @@
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A141" s="28"/>
-      <c r="B141" s="28"/>
+      <c r="A141" s="47"/>
+      <c r="B141" s="47"/>
       <c r="C141" s="7" t="s">
         <v>13</v>
       </c>
@@ -4162,8 +4269,8 @@
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A142" s="28"/>
-      <c r="B142" s="28"/>
+      <c r="A142" s="47"/>
+      <c r="B142" s="47"/>
       <c r="C142" s="13" t="s">
         <v>35</v>
       </c>
@@ -4182,8 +4289,8 @@
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A143" s="28"/>
-      <c r="B143" s="28"/>
+      <c r="A143" s="47"/>
+      <c r="B143" s="47"/>
       <c r="C143" s="7" t="s">
         <v>10</v>
       </c>
@@ -4202,8 +4309,8 @@
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A144" s="28"/>
-      <c r="B144" s="28"/>
+      <c r="A144" s="47"/>
+      <c r="B144" s="47"/>
       <c r="C144" s="13" t="s">
         <v>53</v>
       </c>
@@ -4222,8 +4329,8 @@
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A145" s="28"/>
-      <c r="B145" s="28"/>
+      <c r="A145" s="47"/>
+      <c r="B145" s="47"/>
       <c r="C145" s="7" t="s">
         <v>78</v>
       </c>
@@ -4242,8 +4349,8 @@
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A146" s="28"/>
-      <c r="B146" s="28"/>
+      <c r="A146" s="47"/>
+      <c r="B146" s="47"/>
       <c r="C146" s="13" t="s">
         <v>45</v>
       </c>
@@ -4262,8 +4369,8 @@
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A147" s="28"/>
-      <c r="B147" s="28"/>
+      <c r="A147" s="47"/>
+      <c r="B147" s="47"/>
       <c r="C147" s="7" t="s">
         <v>32</v>
       </c>
@@ -4282,8 +4389,8 @@
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A148" s="28"/>
-      <c r="B148" s="28"/>
+      <c r="A148" s="47"/>
+      <c r="B148" s="47"/>
       <c r="C148" s="13" t="s">
         <v>50</v>
       </c>
@@ -4302,8 +4409,8 @@
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A149" s="28"/>
-      <c r="B149" s="28"/>
+      <c r="A149" s="47"/>
+      <c r="B149" s="47"/>
       <c r="C149" s="7" t="s">
         <v>42</v>
       </c>
@@ -4322,8 +4429,8 @@
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A150" s="28"/>
-      <c r="B150" s="28"/>
+      <c r="A150" s="47"/>
+      <c r="B150" s="47"/>
       <c r="C150" s="13" t="s">
         <v>44</v>
       </c>
@@ -4342,8 +4449,8 @@
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A151" s="28"/>
-      <c r="B151" s="28"/>
+      <c r="A151" s="47"/>
+      <c r="B151" s="47"/>
       <c r="C151" s="7" t="s">
         <v>27</v>
       </c>
@@ -4362,8 +4469,8 @@
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A152" s="28"/>
-      <c r="B152" s="28"/>
+      <c r="A152" s="47"/>
+      <c r="B152" s="47"/>
       <c r="C152" s="13" t="s">
         <v>22</v>
       </c>
@@ -4382,8 +4489,8 @@
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A153" s="28"/>
-      <c r="B153" s="28"/>
+      <c r="A153" s="47"/>
+      <c r="B153" s="47"/>
       <c r="C153" s="7" t="s">
         <v>47</v>
       </c>
@@ -4402,8 +4509,8 @@
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A154" s="28"/>
-      <c r="B154" s="28"/>
+      <c r="A154" s="47"/>
+      <c r="B154" s="47"/>
       <c r="C154" s="13" t="s">
         <v>14</v>
       </c>
@@ -4421,8 +4528,8 @@
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A155" s="28"/>
-      <c r="B155" s="28"/>
+      <c r="A155" s="47"/>
+      <c r="B155" s="47"/>
       <c r="C155" s="7" t="s">
         <v>70</v>
       </c>
@@ -4440,8 +4547,8 @@
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A156" s="28"/>
-      <c r="B156" s="28"/>
+      <c r="A156" s="47"/>
+      <c r="B156" s="47"/>
       <c r="C156" s="13" t="s">
         <v>20</v>
       </c>
@@ -4459,8 +4566,8 @@
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A157" s="28"/>
-      <c r="B157" s="28"/>
+      <c r="A157" s="47"/>
+      <c r="B157" s="47"/>
       <c r="C157" s="7" t="s">
         <v>21</v>
       </c>
@@ -4478,8 +4585,8 @@
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A158" s="28"/>
-      <c r="B158" s="28"/>
+      <c r="A158" s="47"/>
+      <c r="B158" s="47"/>
       <c r="C158" s="13" t="s">
         <v>25</v>
       </c>
@@ -4497,8 +4604,8 @@
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A159" s="28"/>
-      <c r="B159" s="28"/>
+      <c r="A159" s="47"/>
+      <c r="B159" s="47"/>
       <c r="C159" s="7" t="s">
         <v>26</v>
       </c>
@@ -4516,8 +4623,8 @@
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A160" s="28"/>
-      <c r="B160" s="28"/>
+      <c r="A160" s="47"/>
+      <c r="B160" s="47"/>
       <c r="C160" s="13" t="s">
         <v>72</v>
       </c>
@@ -4535,8 +4642,8 @@
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A161" s="28"/>
-      <c r="B161" s="28"/>
+      <c r="A161" s="47"/>
+      <c r="B161" s="47"/>
       <c r="C161" s="7" t="s">
         <v>16</v>
       </c>
@@ -4554,8 +4661,8 @@
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A162" s="28"/>
-      <c r="B162" s="28"/>
+      <c r="A162" s="47"/>
+      <c r="B162" s="47"/>
       <c r="C162" s="13" t="s">
         <v>30</v>
       </c>
@@ -4573,8 +4680,8 @@
       </c>
     </row>
     <row r="163" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A163" s="29"/>
-      <c r="B163" s="29"/>
+      <c r="A163" s="48"/>
+      <c r="B163" s="48"/>
       <c r="C163" s="10" t="s">
         <v>68</v>
       </c>
@@ -4612,13 +4719,2803 @@
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B50C73E3-F1E2-4C38-8160-12F4EB25E464}">
+  <dimension ref="A1:G163"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="Q159" sqref="Q159"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.7265625" style="1"/>
+    <col min="7" max="7" width="14.1796875" style="44" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="21">
+        <v>1979</v>
+      </c>
+      <c r="E1" s="21">
+        <v>1999</v>
+      </c>
+      <c r="F1" s="21">
+        <v>2019</v>
+      </c>
+      <c r="G1" s="34" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="33">
+        <v>0.47368421052631599</v>
+      </c>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="G2" s="35" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="47"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="20">
+        <v>0.68421052631578905</v>
+      </c>
+      <c r="E3" s="20">
+        <v>0.22222222222222199</v>
+      </c>
+      <c r="F3" s="20">
+        <v>0.214285714285714</v>
+      </c>
+      <c r="G3" s="36" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="47"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="27">
+        <v>3.2105263157894699</v>
+      </c>
+      <c r="E4" s="27">
+        <v>1.5</v>
+      </c>
+      <c r="F4" s="27">
+        <v>1.28571428571429</v>
+      </c>
+      <c r="G4" s="37" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="47"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="20">
+        <v>1.1052631578947401</v>
+      </c>
+      <c r="E5" s="20">
+        <v>1.1666666666666701</v>
+      </c>
+      <c r="F5" s="20">
+        <v>0.60714285714285698</v>
+      </c>
+      <c r="G5" s="36" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="47"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" s="27">
+        <v>5.2631578947368397E-2</v>
+      </c>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="G6" s="37" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="47"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="20">
+        <v>0.36842105263157898</v>
+      </c>
+      <c r="E7" s="20">
+        <v>2.2777777777777799</v>
+      </c>
+      <c r="F7" s="20">
+        <v>1.78571428571429</v>
+      </c>
+      <c r="G7" s="36" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="47"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="F8" s="27">
+        <v>0.214285714285714</v>
+      </c>
+      <c r="G8" s="37" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="47"/>
+      <c r="B9" s="47"/>
+      <c r="C9" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="G9" s="38" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="47"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27">
+        <v>5.5555555555555601E-2</v>
+      </c>
+      <c r="F10" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="G10" s="37" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="47"/>
+      <c r="B11" s="48"/>
+      <c r="C11" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="F11" s="29"/>
+      <c r="G11" s="39"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="47"/>
+      <c r="B12" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="30">
+        <v>0.157894736842105</v>
+      </c>
+      <c r="E12" s="30">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="F12" s="30"/>
+      <c r="G12" s="40" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="47"/>
+      <c r="B13" s="47"/>
+      <c r="C13" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="27">
+        <v>5.2631578947368397E-2</v>
+      </c>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="47"/>
+      <c r="B14" s="47"/>
+      <c r="C14" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="20">
+        <v>0.26315789473684198</v>
+      </c>
+      <c r="E14" s="20">
+        <v>0.22222222222222199</v>
+      </c>
+      <c r="F14" s="20"/>
+      <c r="G14" s="37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="47"/>
+      <c r="B15" s="47"/>
+      <c r="C15" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="27">
+        <v>1.3684210526315801</v>
+      </c>
+      <c r="E15" s="27">
+        <v>1.1666666666666701</v>
+      </c>
+      <c r="F15" s="27"/>
+      <c r="G15" s="37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="47"/>
+      <c r="B16" s="47"/>
+      <c r="C16" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="20">
+        <v>0.26315789473684198</v>
+      </c>
+      <c r="E16" s="20">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="F16" s="20"/>
+      <c r="G16" s="37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" s="47"/>
+      <c r="B17" s="47"/>
+      <c r="C17" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="27">
+        <v>0.21052631578947401</v>
+      </c>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" s="47"/>
+      <c r="B18" s="47"/>
+      <c r="C18" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="20">
+        <v>0.63157894736842102</v>
+      </c>
+      <c r="E18" s="20">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="F18" s="20"/>
+      <c r="G18" s="37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" s="47"/>
+      <c r="B19" s="47"/>
+      <c r="C19" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="27">
+        <v>0.105263157894737</v>
+      </c>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" s="47"/>
+      <c r="B20" s="47"/>
+      <c r="C20" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="20">
+        <v>0.63157894736842102</v>
+      </c>
+      <c r="E20" s="20">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="F20" s="20"/>
+      <c r="G20" s="37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" s="47"/>
+      <c r="B21" s="47"/>
+      <c r="C21" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="27">
+        <v>0.94736842105263197</v>
+      </c>
+      <c r="E21" s="27">
+        <v>0.22222222222222199</v>
+      </c>
+      <c r="F21" s="27">
+        <v>7.1428571428571397E-2</v>
+      </c>
+      <c r="G21" s="37" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" s="47"/>
+      <c r="B22" s="47"/>
+      <c r="C22" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="20">
+        <v>0.84210526315789502</v>
+      </c>
+      <c r="E22" s="20">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="F22" s="20">
+        <v>0.14285714285714299</v>
+      </c>
+      <c r="G22" s="36" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23" s="47"/>
+      <c r="B23" s="47"/>
+      <c r="C23" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D23" s="27">
+        <v>0.94736842105263197</v>
+      </c>
+      <c r="E23" s="27">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="F23" s="27">
+        <v>0.17857142857142899</v>
+      </c>
+      <c r="G23" s="37" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24" s="47"/>
+      <c r="B24" s="47"/>
+      <c r="C24" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" s="20">
+        <v>0.157894736842105</v>
+      </c>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20">
+        <v>7.1428571428571397E-2</v>
+      </c>
+      <c r="G24" s="36" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25" s="47"/>
+      <c r="B25" s="47"/>
+      <c r="C25" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="27">
+        <v>0.63157894736842102</v>
+      </c>
+      <c r="E25" s="27">
+        <v>0.77777777777777801</v>
+      </c>
+      <c r="F25" s="27">
+        <v>0.39285714285714302</v>
+      </c>
+      <c r="G25" s="37" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26" s="47"/>
+      <c r="B26" s="47"/>
+      <c r="C26" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D26" s="20">
+        <v>0.47368421052631599</v>
+      </c>
+      <c r="E26" s="20">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="F26" s="20">
+        <v>0.32142857142857101</v>
+      </c>
+      <c r="G26" s="36" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27" s="47"/>
+      <c r="B27" s="47"/>
+      <c r="C27" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" s="27">
+        <v>5.2631578947368397E-2</v>
+      </c>
+      <c r="E27" s="27">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="F27" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="G27" s="37" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28" s="47"/>
+      <c r="B28" s="47"/>
+      <c r="C28" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" s="20">
+        <v>5.2631578947368397E-2</v>
+      </c>
+      <c r="E28" s="20">
+        <v>5.5555555555555601E-2</v>
+      </c>
+      <c r="F28" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="G28" s="36" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A29" s="47"/>
+      <c r="B29" s="47"/>
+      <c r="C29" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D29" s="27">
+        <v>3.8421052631578898</v>
+      </c>
+      <c r="E29" s="27">
+        <v>3.0555555555555598</v>
+      </c>
+      <c r="F29" s="27">
+        <v>3</v>
+      </c>
+      <c r="G29" s="37" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A30" s="47"/>
+      <c r="B30" s="47"/>
+      <c r="C30" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D30" s="20">
+        <v>0.52631578947368396</v>
+      </c>
+      <c r="E30" s="20">
+        <v>0.22222222222222199</v>
+      </c>
+      <c r="F30" s="20">
+        <v>0.57142857142857095</v>
+      </c>
+      <c r="G30" s="36" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A31" s="47"/>
+      <c r="B31" s="47"/>
+      <c r="C31" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D31" s="27">
+        <v>0.26315789473684198</v>
+      </c>
+      <c r="E31" s="27">
+        <v>0.38888888888888901</v>
+      </c>
+      <c r="F31" s="27">
+        <v>0.28571428571428598</v>
+      </c>
+      <c r="G31" s="37" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A32" s="47"/>
+      <c r="B32" s="47"/>
+      <c r="C32" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D32" s="20">
+        <v>5.2631578947368397E-2</v>
+      </c>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20">
+        <v>7.1428571428571397E-2</v>
+      </c>
+      <c r="G32" s="36" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A33" s="47"/>
+      <c r="B33" s="47"/>
+      <c r="C33" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" s="27">
+        <v>0.47368421052631599</v>
+      </c>
+      <c r="E33" s="27">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="F33" s="27">
+        <v>1</v>
+      </c>
+      <c r="G33" s="37" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A34" s="47"/>
+      <c r="B34" s="47"/>
+      <c r="C34" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D34" s="20">
+        <v>5.2631578947368397E-2</v>
+      </c>
+      <c r="E34" s="20">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="F34" s="20">
+        <v>0.14285714285714299</v>
+      </c>
+      <c r="G34" s="36" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A35" s="47"/>
+      <c r="B35" s="47"/>
+      <c r="C35" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D35" s="27">
+        <v>0.26315789473684198</v>
+      </c>
+      <c r="E35" s="27">
+        <v>1</v>
+      </c>
+      <c r="F35" s="27">
+        <v>1.0714285714285701</v>
+      </c>
+      <c r="G35" s="37" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A36" s="47"/>
+      <c r="B36" s="47"/>
+      <c r="C36" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" s="20"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="20">
+        <v>0.64285714285714302</v>
+      </c>
+      <c r="G36" s="37" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A37" s="47"/>
+      <c r="B37" s="47"/>
+      <c r="C37" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D37" s="27"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="27">
+        <v>0.39285714285714302</v>
+      </c>
+      <c r="G37" s="37" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A38" s="47"/>
+      <c r="B38" s="47"/>
+      <c r="C38" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D38" s="20"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="G38" s="37" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A39" s="47"/>
+      <c r="B39" s="47"/>
+      <c r="C39" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D39" s="27"/>
+      <c r="E39" s="27">
+        <v>0.44444444444444398</v>
+      </c>
+      <c r="F39" s="27">
+        <v>0.32142857142857101</v>
+      </c>
+      <c r="G39" s="37" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A40" s="47"/>
+      <c r="B40" s="47"/>
+      <c r="C40" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="G40" s="37" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A41" s="47"/>
+      <c r="B41" s="47"/>
+      <c r="C41" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D41" s="27"/>
+      <c r="E41" s="27">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="F41" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="G41" s="37" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A42" s="47"/>
+      <c r="B42" s="47"/>
+      <c r="C42" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D42" s="20"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="20">
+        <v>7.1428571428571397E-2</v>
+      </c>
+      <c r="G42" s="37" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A43" s="47"/>
+      <c r="B43" s="47"/>
+      <c r="C43" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D43" s="27"/>
+      <c r="E43" s="27">
+        <v>0.61111111111111105</v>
+      </c>
+      <c r="F43" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="G43" s="37" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A44" s="47"/>
+      <c r="B44" s="47"/>
+      <c r="C44" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D44" s="20"/>
+      <c r="E44" s="20"/>
+      <c r="F44" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="G44" s="37" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A45" s="47"/>
+      <c r="B45" s="47"/>
+      <c r="C45" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D45" s="27"/>
+      <c r="E45" s="27">
+        <v>0.27777777777777801</v>
+      </c>
+      <c r="F45" s="27">
+        <v>0.25</v>
+      </c>
+      <c r="G45" s="37" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A46" s="47"/>
+      <c r="B46" s="47"/>
+      <c r="C46" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D46" s="20"/>
+      <c r="E46" s="20">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="F46" s="20"/>
+      <c r="G46" s="36"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A47" s="47"/>
+      <c r="B47" s="47"/>
+      <c r="C47" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D47" s="27"/>
+      <c r="E47" s="27">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="F47" s="27"/>
+      <c r="G47" s="37"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A48" s="47"/>
+      <c r="B48" s="47"/>
+      <c r="C48" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D48" s="20"/>
+      <c r="E48" s="20">
+        <v>5.5555555555555601E-2</v>
+      </c>
+      <c r="F48" s="20"/>
+      <c r="G48" s="36"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A49" s="47"/>
+      <c r="B49" s="47"/>
+      <c r="C49" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D49" s="27"/>
+      <c r="E49" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="F49" s="27"/>
+      <c r="G49" s="37"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A50" s="47"/>
+      <c r="B50" s="47"/>
+      <c r="C50" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D50" s="27"/>
+      <c r="E50" s="27">
+        <v>0.27777777777777801</v>
+      </c>
+      <c r="F50" s="27"/>
+      <c r="G50" s="37"/>
+    </row>
+    <row r="51" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A51" s="48"/>
+      <c r="B51" s="48"/>
+      <c r="C51" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D51" s="29"/>
+      <c r="E51" s="29">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="F51" s="29"/>
+      <c r="G51" s="39"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A52" s="19"/>
+      <c r="B52" s="19"/>
+      <c r="C52" s="7"/>
+      <c r="D52" s="8"/>
+      <c r="E52" s="8"/>
+      <c r="F52" s="8"/>
+      <c r="G52" s="41"/>
+    </row>
+    <row r="53" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A53" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C53" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D53" s="21">
+        <v>1979</v>
+      </c>
+      <c r="E53" s="21">
+        <v>1999</v>
+      </c>
+      <c r="F53" s="21">
+        <v>2019</v>
+      </c>
+      <c r="G53" s="34" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A54" s="46" t="s">
+        <v>54</v>
+      </c>
+      <c r="B54" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C54" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="D54" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="E54" s="31"/>
+      <c r="F54" s="31"/>
+      <c r="G54" s="42" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A55" s="47"/>
+      <c r="B55" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D55" s="30">
+        <v>0.31034482758620702</v>
+      </c>
+      <c r="E55" s="30">
+        <v>9.0909090909090898E-2</v>
+      </c>
+      <c r="F55" s="30"/>
+      <c r="G55" s="40" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A56" s="47"/>
+      <c r="B56" s="47"/>
+      <c r="C56" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D56" s="27">
+        <v>0.31034482758620702</v>
+      </c>
+      <c r="E56" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="F56" s="27"/>
+      <c r="G56" s="37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A57" s="47"/>
+      <c r="B57" s="47"/>
+      <c r="C57" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D57" s="20">
+        <v>0.17241379310344801</v>
+      </c>
+      <c r="E57" s="20">
+        <v>0.24242424242424199</v>
+      </c>
+      <c r="F57" s="20">
+        <v>5.5555555555555601E-2</v>
+      </c>
+      <c r="G57" s="36" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A58" s="47"/>
+      <c r="B58" s="47"/>
+      <c r="C58" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D58" s="27">
+        <v>1.55172413793103</v>
+      </c>
+      <c r="E58" s="27">
+        <v>0.90909090909090895</v>
+      </c>
+      <c r="F58" s="27">
+        <v>0.72222222222222199</v>
+      </c>
+      <c r="G58" s="37" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A59" s="47"/>
+      <c r="B59" s="47"/>
+      <c r="C59" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D59" s="20">
+        <v>0.37931034482758602</v>
+      </c>
+      <c r="E59" s="20">
+        <v>0.57575757575757602</v>
+      </c>
+      <c r="F59" s="20">
+        <v>0.44444444444444398</v>
+      </c>
+      <c r="G59" s="36" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A60" s="47"/>
+      <c r="B60" s="47"/>
+      <c r="C60" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D60" s="27">
+        <v>0.34482758620689702</v>
+      </c>
+      <c r="E60" s="27">
+        <v>0.81818181818181801</v>
+      </c>
+      <c r="F60" s="27">
+        <v>0.61111111111111105</v>
+      </c>
+      <c r="G60" s="37" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A61" s="47"/>
+      <c r="B61" s="47"/>
+      <c r="C61" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D61" s="20">
+        <v>6.8965517241379296E-2</v>
+      </c>
+      <c r="E61" s="20">
+        <v>0.15151515151515199</v>
+      </c>
+      <c r="F61" s="20">
+        <v>1.05555555555556</v>
+      </c>
+      <c r="G61" s="36" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A62" s="47"/>
+      <c r="B62" s="47"/>
+      <c r="C62" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D62" s="27"/>
+      <c r="E62" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="F62" s="27">
+        <v>5.5555555555555601E-2</v>
+      </c>
+      <c r="G62" s="37" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A63" s="47"/>
+      <c r="B63" s="47"/>
+      <c r="C63" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D63" s="27"/>
+      <c r="E63" s="27">
+        <v>0.15151515151515199</v>
+      </c>
+      <c r="F63" s="27">
+        <v>0.22222222222222199</v>
+      </c>
+      <c r="G63" s="37" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A64" s="47"/>
+      <c r="B64" s="48"/>
+      <c r="C64" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D64" s="29"/>
+      <c r="E64" s="29"/>
+      <c r="F64" s="29">
+        <v>5.5555555555555601E-2</v>
+      </c>
+      <c r="G64" s="39" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A65" s="47"/>
+      <c r="B65" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D65" s="30">
+        <v>0.10344827586206901</v>
+      </c>
+      <c r="E65" s="30">
+        <v>0.18181818181818199</v>
+      </c>
+      <c r="F65" s="30"/>
+      <c r="G65" s="40" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A66" s="47"/>
+      <c r="B66" s="47"/>
+      <c r="C66" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D66" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="E66" s="27"/>
+      <c r="F66" s="27"/>
+      <c r="G66" s="37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A67" s="47"/>
+      <c r="B67" s="47"/>
+      <c r="C67" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D67" s="20">
+        <v>0.20689655172413801</v>
+      </c>
+      <c r="E67" s="20">
+        <v>0.51515151515151503</v>
+      </c>
+      <c r="F67" s="20"/>
+      <c r="G67" s="37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A68" s="47"/>
+      <c r="B68" s="47"/>
+      <c r="C68" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D68" s="27">
+        <v>0.62068965517241403</v>
+      </c>
+      <c r="E68" s="27">
+        <v>9.0909090909090898E-2</v>
+      </c>
+      <c r="F68" s="27"/>
+      <c r="G68" s="37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A69" s="47"/>
+      <c r="B69" s="47"/>
+      <c r="C69" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D69" s="20">
+        <v>6.8965517241379296E-2</v>
+      </c>
+      <c r="E69" s="20"/>
+      <c r="F69" s="20"/>
+      <c r="G69" s="37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A70" s="47"/>
+      <c r="B70" s="47"/>
+      <c r="C70" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D70" s="27">
+        <v>0.96551724137931005</v>
+      </c>
+      <c r="E70" s="27">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="F70" s="27"/>
+      <c r="G70" s="37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A71" s="47"/>
+      <c r="B71" s="47"/>
+      <c r="C71" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D71" s="20">
+        <v>0.75862068965517204</v>
+      </c>
+      <c r="E71" s="20">
+        <v>9.0909090909090898E-2</v>
+      </c>
+      <c r="F71" s="20"/>
+      <c r="G71" s="37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A72" s="47"/>
+      <c r="B72" s="47"/>
+      <c r="C72" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D72" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="E72" s="27"/>
+      <c r="F72" s="27"/>
+      <c r="G72" s="37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A73" s="47"/>
+      <c r="B73" s="47"/>
+      <c r="C73" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D73" s="20">
+        <v>0.10344827586206901</v>
+      </c>
+      <c r="E73" s="20"/>
+      <c r="F73" s="20"/>
+      <c r="G73" s="37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A74" s="47"/>
+      <c r="B74" s="47"/>
+      <c r="C74" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D74" s="27">
+        <v>0.51724137931034497</v>
+      </c>
+      <c r="E74" s="27">
+        <v>6.0606060606060601E-2</v>
+      </c>
+      <c r="F74" s="27"/>
+      <c r="G74" s="37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A75" s="47"/>
+      <c r="B75" s="47"/>
+      <c r="C75" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D75" s="20">
+        <v>0.13793103448275901</v>
+      </c>
+      <c r="E75" s="20">
+        <v>0.24242424242424199</v>
+      </c>
+      <c r="F75" s="20"/>
+      <c r="G75" s="37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A76" s="47"/>
+      <c r="B76" s="47"/>
+      <c r="C76" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D76" s="27">
+        <v>0.17241379310344801</v>
+      </c>
+      <c r="E76" s="27"/>
+      <c r="F76" s="27"/>
+      <c r="G76" s="37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A77" s="47"/>
+      <c r="B77" s="47"/>
+      <c r="C77" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D77" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="E77" s="20"/>
+      <c r="F77" s="20"/>
+      <c r="G77" s="37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A78" s="47"/>
+      <c r="B78" s="47"/>
+      <c r="C78" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D78" s="27">
+        <v>0.17241379310344801</v>
+      </c>
+      <c r="E78" s="27">
+        <v>0.30303030303030298</v>
+      </c>
+      <c r="F78" s="27"/>
+      <c r="G78" s="37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A79" s="47"/>
+      <c r="B79" s="47"/>
+      <c r="C79" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D79" s="20">
+        <v>0.20689655172413801</v>
+      </c>
+      <c r="E79" s="20">
+        <v>3.03030303030303E-2</v>
+      </c>
+      <c r="F79" s="20"/>
+      <c r="G79" s="37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A80" s="47"/>
+      <c r="B80" s="47"/>
+      <c r="C80" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D80" s="27">
+        <v>0.55172413793103403</v>
+      </c>
+      <c r="E80" s="27">
+        <v>1.72727272727273</v>
+      </c>
+      <c r="F80" s="27"/>
+      <c r="G80" s="37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A81" s="47"/>
+      <c r="B81" s="47"/>
+      <c r="C81" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D81" s="20">
+        <v>0.31034482758620702</v>
+      </c>
+      <c r="E81" s="20"/>
+      <c r="F81" s="20"/>
+      <c r="G81" s="37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A82" s="47"/>
+      <c r="B82" s="47"/>
+      <c r="C82" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D82" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="E82" s="27"/>
+      <c r="F82" s="27"/>
+      <c r="G82" s="37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A83" s="47"/>
+      <c r="B83" s="47"/>
+      <c r="C83" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D83" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="E83" s="20">
+        <v>0.15151515151515199</v>
+      </c>
+      <c r="F83" s="20"/>
+      <c r="G83" s="37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A84" s="47"/>
+      <c r="B84" s="47"/>
+      <c r="C84" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="D84" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="E84" s="27"/>
+      <c r="F84" s="27"/>
+      <c r="G84" s="37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A85" s="47"/>
+      <c r="B85" s="47"/>
+      <c r="C85" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D85" s="20">
+        <v>0.13793103448275901</v>
+      </c>
+      <c r="E85" s="20">
+        <v>0.15151515151515199</v>
+      </c>
+      <c r="F85" s="20"/>
+      <c r="G85" s="37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A86" s="47"/>
+      <c r="B86" s="47"/>
+      <c r="C86" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="D86" s="27">
+        <v>0.58620689655172398</v>
+      </c>
+      <c r="E86" s="27">
+        <v>0.24242424242424199</v>
+      </c>
+      <c r="F86" s="27"/>
+      <c r="G86" s="37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A87" s="47"/>
+      <c r="B87" s="47"/>
+      <c r="C87" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D87" s="20">
+        <v>0.68965517241379304</v>
+      </c>
+      <c r="E87" s="20">
+        <v>0.54545454545454497</v>
+      </c>
+      <c r="F87" s="20"/>
+      <c r="G87" s="37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A88" s="47"/>
+      <c r="B88" s="47"/>
+      <c r="C88" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D88" s="27">
+        <v>1.86206896551724</v>
+      </c>
+      <c r="E88" s="27">
+        <v>1.3333333333333299</v>
+      </c>
+      <c r="F88" s="27">
+        <v>5.5555555555555601E-2</v>
+      </c>
+      <c r="G88" s="37" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A89" s="47"/>
+      <c r="B89" s="47"/>
+      <c r="C89" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D89" s="20">
+        <v>0.65517241379310298</v>
+      </c>
+      <c r="E89" s="20">
+        <v>0.39393939393939398</v>
+      </c>
+      <c r="F89" s="20">
+        <v>5.5555555555555601E-2</v>
+      </c>
+      <c r="G89" s="36" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A90" s="47"/>
+      <c r="B90" s="47"/>
+      <c r="C90" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D90" s="27">
+        <v>1</v>
+      </c>
+      <c r="E90" s="27">
+        <v>0.39393939393939398</v>
+      </c>
+      <c r="F90" s="27">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="G90" s="37" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A91" s="47"/>
+      <c r="B91" s="47"/>
+      <c r="C91" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D91" s="20">
+        <v>0.75862068965517204</v>
+      </c>
+      <c r="E91" s="20">
+        <v>1.4242424242424201</v>
+      </c>
+      <c r="F91" s="20">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="G91" s="36" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A92" s="47"/>
+      <c r="B92" s="47"/>
+      <c r="C92" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D92" s="27">
+        <v>0.48275862068965503</v>
+      </c>
+      <c r="E92" s="27">
+        <v>0.63636363636363602</v>
+      </c>
+      <c r="F92" s="27">
+        <v>0.22222222222222199</v>
+      </c>
+      <c r="G92" s="37" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A93" s="47"/>
+      <c r="B93" s="47"/>
+      <c r="C93" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D93" s="20">
+        <v>0.41379310344827602</v>
+      </c>
+      <c r="E93" s="20">
+        <v>0.18181818181818199</v>
+      </c>
+      <c r="F93" s="20">
+        <v>0.22222222222222199</v>
+      </c>
+      <c r="G93" s="36" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A94" s="47"/>
+      <c r="B94" s="47"/>
+      <c r="C94" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D94" s="27">
+        <v>0.10344827586206901</v>
+      </c>
+      <c r="E94" s="27">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="F94" s="27">
+        <v>5.5555555555555601E-2</v>
+      </c>
+      <c r="G94" s="37" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A95" s="47"/>
+      <c r="B95" s="47"/>
+      <c r="C95" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D95" s="20">
+        <v>0.68965517241379304</v>
+      </c>
+      <c r="E95" s="20">
+        <v>0.36363636363636398</v>
+      </c>
+      <c r="F95" s="20">
+        <v>0.44444444444444398</v>
+      </c>
+      <c r="G95" s="36" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A96" s="47"/>
+      <c r="B96" s="47"/>
+      <c r="C96" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="D96" s="27">
+        <v>0.17241379310344801</v>
+      </c>
+      <c r="E96" s="27"/>
+      <c r="F96" s="27">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="G96" s="37" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A97" s="47"/>
+      <c r="B97" s="47"/>
+      <c r="C97" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D97" s="20">
+        <v>0.62068965517241403</v>
+      </c>
+      <c r="E97" s="20">
+        <v>0.36363636363636398</v>
+      </c>
+      <c r="F97" s="20">
+        <v>0.44444444444444398</v>
+      </c>
+      <c r="G97" s="36" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A98" s="47"/>
+      <c r="B98" s="47"/>
+      <c r="C98" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D98" s="27">
+        <v>6.8965517241379296E-2</v>
+      </c>
+      <c r="E98" s="27">
+        <v>0.15151515151515199</v>
+      </c>
+      <c r="F98" s="27">
+        <v>5.5555555555555601E-2</v>
+      </c>
+      <c r="G98" s="37" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A99" s="47"/>
+      <c r="B99" s="47"/>
+      <c r="C99" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D99" s="20">
+        <v>0.55172413793103403</v>
+      </c>
+      <c r="E99" s="20">
+        <v>0.18181818181818199</v>
+      </c>
+      <c r="F99" s="20">
+        <v>0.55555555555555602</v>
+      </c>
+      <c r="G99" s="36" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A100" s="47"/>
+      <c r="B100" s="47"/>
+      <c r="C100" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D100" s="27">
+        <v>6.8965517241379296E-2</v>
+      </c>
+      <c r="E100" s="27">
+        <v>0.15151515151515199</v>
+      </c>
+      <c r="F100" s="27">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="G100" s="37" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A101" s="47"/>
+      <c r="B101" s="47"/>
+      <c r="C101" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D101" s="20">
+        <v>0.27586206896551702</v>
+      </c>
+      <c r="E101" s="20">
+        <v>0.42424242424242398</v>
+      </c>
+      <c r="F101" s="20">
+        <v>0.61111111111111105</v>
+      </c>
+      <c r="G101" s="36" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A102" s="47"/>
+      <c r="B102" s="47"/>
+      <c r="C102" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D102" s="27"/>
+      <c r="E102" s="27"/>
+      <c r="F102" s="27">
+        <v>0.38888888888888901</v>
+      </c>
+      <c r="G102" s="37" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A103" s="47"/>
+      <c r="B103" s="47"/>
+      <c r="C103" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D103" s="20"/>
+      <c r="E103" s="20"/>
+      <c r="F103" s="20">
+        <v>5.5555555555555601E-2</v>
+      </c>
+      <c r="G103" s="37" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A104" s="47"/>
+      <c r="B104" s="47"/>
+      <c r="C104" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D104" s="27"/>
+      <c r="E104" s="27"/>
+      <c r="F104" s="27">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="G104" s="37" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A105" s="47"/>
+      <c r="B105" s="47"/>
+      <c r="C105" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D105" s="20"/>
+      <c r="E105" s="20"/>
+      <c r="F105" s="20">
+        <v>0.22222222222222199</v>
+      </c>
+      <c r="G105" s="37" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A106" s="47"/>
+      <c r="B106" s="47"/>
+      <c r="C106" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D106" s="27"/>
+      <c r="E106" s="27"/>
+      <c r="F106" s="27">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="G106" s="37" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A107" s="47"/>
+      <c r="B107" s="47"/>
+      <c r="C107" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D107" s="20"/>
+      <c r="E107" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="F107" s="20"/>
+      <c r="G107" s="36"/>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A108" s="47"/>
+      <c r="B108" s="47"/>
+      <c r="C108" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D108" s="27"/>
+      <c r="E108" s="27">
+        <v>6.0606060606060601E-2</v>
+      </c>
+      <c r="F108" s="27"/>
+      <c r="G108" s="37"/>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A109" s="47"/>
+      <c r="B109" s="47"/>
+      <c r="C109" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D109" s="20"/>
+      <c r="E109" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="F109" s="20"/>
+      <c r="G109" s="36"/>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A110" s="47"/>
+      <c r="B110" s="47"/>
+      <c r="C110" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D110" s="27"/>
+      <c r="E110" s="27">
+        <v>9.0909090909090898E-2</v>
+      </c>
+      <c r="F110" s="27"/>
+      <c r="G110" s="37"/>
+    </row>
+    <row r="111" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A111" s="48"/>
+      <c r="B111" s="48"/>
+      <c r="C111" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D111" s="29"/>
+      <c r="E111" s="45" t="s">
+        <v>79</v>
+      </c>
+      <c r="F111" s="29"/>
+      <c r="G111" s="39"/>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A112" s="3"/>
+      <c r="B112" s="19"/>
+      <c r="C112" s="7"/>
+      <c r="D112" s="8"/>
+      <c r="E112" s="8"/>
+      <c r="F112" s="8"/>
+      <c r="G112" s="41"/>
+    </row>
+    <row r="113" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A113" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B113" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C113" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D113" s="21">
+        <v>1979</v>
+      </c>
+      <c r="E113" s="21">
+        <v>1999</v>
+      </c>
+      <c r="F113" s="21">
+        <v>2019</v>
+      </c>
+      <c r="G113" s="34" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A114" s="46" t="s">
+        <v>69</v>
+      </c>
+      <c r="B114" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C114" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="D114" s="31"/>
+      <c r="E114" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="F114" s="31"/>
+      <c r="G114" s="42"/>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A115" s="47"/>
+      <c r="B115" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="C115" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D115" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="E115" s="30"/>
+      <c r="F115" s="30"/>
+      <c r="G115" s="40" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A116" s="47"/>
+      <c r="B116" s="47"/>
+      <c r="C116" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D116" s="27">
+        <v>0.29411764705882398</v>
+      </c>
+      <c r="E116" s="27">
+        <v>0.16129032258064499</v>
+      </c>
+      <c r="F116" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="G116" s="37" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A117" s="47"/>
+      <c r="B117" s="47"/>
+      <c r="C117" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D117" s="20">
+        <v>1.8529411764705901</v>
+      </c>
+      <c r="E117" s="20">
+        <v>2.32258064516129</v>
+      </c>
+      <c r="F117" s="20">
+        <v>1.25</v>
+      </c>
+      <c r="G117" s="36" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A118" s="47"/>
+      <c r="B118" s="47"/>
+      <c r="C118" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D118" s="27">
+        <v>0.26470588235294101</v>
+      </c>
+      <c r="E118" s="27">
+        <v>0.25806451612903197</v>
+      </c>
+      <c r="F118" s="27">
+        <v>0.39285714285714302</v>
+      </c>
+      <c r="G118" s="37" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A119" s="47"/>
+      <c r="B119" s="47"/>
+      <c r="C119" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D119" s="20">
+        <v>8.8235294117647106E-2</v>
+      </c>
+      <c r="E119" s="20">
+        <v>9.6774193548387094E-2</v>
+      </c>
+      <c r="F119" s="20">
+        <v>0.17857142857142899</v>
+      </c>
+      <c r="G119" s="36" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A120" s="47"/>
+      <c r="B120" s="47"/>
+      <c r="C120" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D120" s="27"/>
+      <c r="E120" s="27">
+        <v>0.12903225806451599</v>
+      </c>
+      <c r="F120" s="27">
+        <v>0.25</v>
+      </c>
+      <c r="G120" s="37" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A121" s="47"/>
+      <c r="B121" s="47"/>
+      <c r="C121" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D121" s="20"/>
+      <c r="E121" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="F121" s="20">
+        <v>0.107142857142857</v>
+      </c>
+      <c r="G121" s="37" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A122" s="47"/>
+      <c r="B122" s="47"/>
+      <c r="C122" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D122" s="27"/>
+      <c r="E122" s="27">
+        <v>0.16129032258064499</v>
+      </c>
+      <c r="F122" s="27">
+        <v>0.53571428571428603</v>
+      </c>
+      <c r="G122" s="37" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A123" s="47"/>
+      <c r="B123" s="47"/>
+      <c r="C123" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D123" s="27"/>
+      <c r="E123" s="27"/>
+      <c r="F123" s="27">
+        <v>7.1428571428571397E-2</v>
+      </c>
+      <c r="G123" s="37" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A124" s="47"/>
+      <c r="B124" s="48"/>
+      <c r="C124" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D124" s="29"/>
+      <c r="E124" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="F124" s="29"/>
+      <c r="G124" s="39"/>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A125" s="47"/>
+      <c r="B125" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="C125" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D125" s="30">
+        <v>0.35294117647058798</v>
+      </c>
+      <c r="E125" s="30">
+        <v>6.4516129032258104E-2</v>
+      </c>
+      <c r="F125" s="30"/>
+      <c r="G125" s="40" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A126" s="47"/>
+      <c r="B126" s="47"/>
+      <c r="C126" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D126" s="27">
+        <v>0.20588235294117599</v>
+      </c>
+      <c r="E126" s="27"/>
+      <c r="F126" s="27"/>
+      <c r="G126" s="37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A127" s="47"/>
+      <c r="B127" s="47"/>
+      <c r="C127" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D127" s="20">
+        <v>0.17647058823529399</v>
+      </c>
+      <c r="E127" s="20">
+        <v>0.19354838709677399</v>
+      </c>
+      <c r="F127" s="20"/>
+      <c r="G127" s="37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A128" s="47"/>
+      <c r="B128" s="47"/>
+      <c r="C128" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D128" s="27">
+        <v>5.8823529411764698E-2</v>
+      </c>
+      <c r="E128" s="27">
+        <v>9.6774193548387094E-2</v>
+      </c>
+      <c r="F128" s="27"/>
+      <c r="G128" s="37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A129" s="47"/>
+      <c r="B129" s="47"/>
+      <c r="C129" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D129" s="20">
+        <v>8.8235294117647106E-2</v>
+      </c>
+      <c r="E129" s="20"/>
+      <c r="F129" s="20"/>
+      <c r="G129" s="37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A130" s="47"/>
+      <c r="B130" s="47"/>
+      <c r="C130" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D130" s="27">
+        <v>0.70588235294117696</v>
+      </c>
+      <c r="E130" s="27">
+        <v>0.38709677419354799</v>
+      </c>
+      <c r="F130" s="27"/>
+      <c r="G130" s="37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A131" s="47"/>
+      <c r="B131" s="47"/>
+      <c r="C131" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D131" s="20">
+        <v>8.8235294117647106E-2</v>
+      </c>
+      <c r="E131" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="F131" s="20"/>
+      <c r="G131" s="37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A132" s="47"/>
+      <c r="B132" s="47"/>
+      <c r="C132" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D132" s="27">
+        <v>1</v>
+      </c>
+      <c r="E132" s="27">
+        <v>0.225806451612903</v>
+      </c>
+      <c r="F132" s="27"/>
+      <c r="G132" s="37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A133" s="47"/>
+      <c r="B133" s="47"/>
+      <c r="C133" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D133" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="E133" s="20"/>
+      <c r="F133" s="20"/>
+      <c r="G133" s="37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A134" s="47"/>
+      <c r="B134" s="47"/>
+      <c r="C134" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D134" s="27">
+        <v>0.58823529411764697</v>
+      </c>
+      <c r="E134" s="27">
+        <v>0.19354838709677399</v>
+      </c>
+      <c r="F134" s="27"/>
+      <c r="G134" s="37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A135" s="47"/>
+      <c r="B135" s="47"/>
+      <c r="C135" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D135" s="20">
+        <v>1.0882352941176501</v>
+      </c>
+      <c r="E135" s="20">
+        <v>0.483870967741935</v>
+      </c>
+      <c r="F135" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="G135" s="37" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A136" s="47"/>
+      <c r="B136" s="47"/>
+      <c r="C136" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D136" s="27">
+        <v>0.88235294117647101</v>
+      </c>
+      <c r="E136" s="27">
+        <v>0.58064516129032295</v>
+      </c>
+      <c r="F136" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="G136" s="37" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A137" s="47"/>
+      <c r="B137" s="47"/>
+      <c r="C137" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D137" s="20">
+        <v>0.70588235294117696</v>
+      </c>
+      <c r="E137" s="20">
+        <v>9.6774193548387094E-2</v>
+      </c>
+      <c r="F137" s="20">
+        <v>0.107142857142857</v>
+      </c>
+      <c r="G137" s="37" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A138" s="47"/>
+      <c r="B138" s="47"/>
+      <c r="C138" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D138" s="27">
+        <v>0.41176470588235298</v>
+      </c>
+      <c r="E138" s="27">
+        <v>0.12903225806451599</v>
+      </c>
+      <c r="F138" s="27">
+        <v>7.1428571428571397E-2</v>
+      </c>
+      <c r="G138" s="37" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A139" s="47"/>
+      <c r="B139" s="47"/>
+      <c r="C139" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D139" s="20">
+        <v>0.41176470588235298</v>
+      </c>
+      <c r="E139" s="20">
+        <v>9.6774193548387094E-2</v>
+      </c>
+      <c r="F139" s="20">
+        <v>0.107142857142857</v>
+      </c>
+      <c r="G139" s="37" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A140" s="47"/>
+      <c r="B140" s="47"/>
+      <c r="C140" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D140" s="27">
+        <v>0.47058823529411797</v>
+      </c>
+      <c r="E140" s="27">
+        <v>0.12903225806451599</v>
+      </c>
+      <c r="F140" s="27">
+        <v>0.214285714285714</v>
+      </c>
+      <c r="G140" s="37" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A141" s="47"/>
+      <c r="B141" s="47"/>
+      <c r="C141" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D141" s="20">
+        <v>0.79411764705882304</v>
+      </c>
+      <c r="E141" s="20">
+        <v>0.35483870967741898</v>
+      </c>
+      <c r="F141" s="20">
+        <v>0.39285714285714302</v>
+      </c>
+      <c r="G141" s="37" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A142" s="47"/>
+      <c r="B142" s="47"/>
+      <c r="C142" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D142" s="27">
+        <v>0.32352941176470601</v>
+      </c>
+      <c r="E142" s="27">
+        <v>0.67741935483870996</v>
+      </c>
+      <c r="F142" s="27">
+        <v>0.17857142857142899</v>
+      </c>
+      <c r="G142" s="37" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A143" s="47"/>
+      <c r="B143" s="47"/>
+      <c r="C143" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D143" s="20">
+        <v>2.97058823529412</v>
+      </c>
+      <c r="E143" s="20">
+        <v>3.0322580645161299</v>
+      </c>
+      <c r="F143" s="20">
+        <v>1.9285714285714299</v>
+      </c>
+      <c r="G143" s="37" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A144" s="47"/>
+      <c r="B144" s="47"/>
+      <c r="C144" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D144" s="27">
+        <v>0.58823529411764697</v>
+      </c>
+      <c r="E144" s="27">
+        <v>0.35483870967741898</v>
+      </c>
+      <c r="F144" s="27">
+        <v>0.42857142857142899</v>
+      </c>
+      <c r="G144" s="37" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A145" s="47"/>
+      <c r="B145" s="47"/>
+      <c r="C145" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D145" s="20">
+        <v>0.29411764705882398</v>
+      </c>
+      <c r="E145" s="20">
+        <v>0.12903225806451599</v>
+      </c>
+      <c r="F145" s="20">
+        <v>0.25</v>
+      </c>
+      <c r="G145" s="37" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A146" s="47"/>
+      <c r="B146" s="47"/>
+      <c r="C146" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D146" s="27">
+        <v>0.11764705882352899</v>
+      </c>
+      <c r="E146" s="27">
+        <v>0.16129032258064499</v>
+      </c>
+      <c r="F146" s="27">
+        <v>0.107142857142857</v>
+      </c>
+      <c r="G146" s="37" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A147" s="47"/>
+      <c r="B147" s="47"/>
+      <c r="C147" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D147" s="20">
+        <v>8.8235294117647106E-2</v>
+      </c>
+      <c r="E147" s="20"/>
+      <c r="F147" s="20">
+        <v>0.107142857142857</v>
+      </c>
+      <c r="G147" s="36" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A148" s="47"/>
+      <c r="B148" s="47"/>
+      <c r="C148" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D148" s="27">
+        <v>8.8235294117647106E-2</v>
+      </c>
+      <c r="E148" s="27">
+        <v>9.6774193548387094E-2</v>
+      </c>
+      <c r="F148" s="27">
+        <v>0.214285714285714</v>
+      </c>
+      <c r="G148" s="37" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A149" s="47"/>
+      <c r="B149" s="47"/>
+      <c r="C149" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D149" s="20">
+        <v>0.29411764705882398</v>
+      </c>
+      <c r="E149" s="20">
+        <v>0.74193548387096797</v>
+      </c>
+      <c r="F149" s="20">
+        <v>0.78571428571428603</v>
+      </c>
+      <c r="G149" s="36" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A150" s="47"/>
+      <c r="B150" s="47"/>
+      <c r="C150" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D150" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="E150" s="27"/>
+      <c r="F150" s="27">
+        <v>0.107142857142857</v>
+      </c>
+      <c r="G150" s="37" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A151" s="47"/>
+      <c r="B151" s="47"/>
+      <c r="C151" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D151" s="20">
+        <v>8.8235294117647106E-2</v>
+      </c>
+      <c r="E151" s="20">
+        <v>0.25806451612903197</v>
+      </c>
+      <c r="F151" s="20">
+        <v>0.46428571428571402</v>
+      </c>
+      <c r="G151" s="36" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A152" s="47"/>
+      <c r="B152" s="47"/>
+      <c r="C152" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D152" s="27">
+        <v>0.14705882352941199</v>
+      </c>
+      <c r="E152" s="27">
+        <v>1.06451612903226</v>
+      </c>
+      <c r="F152" s="27">
+        <v>0.85714285714285698</v>
+      </c>
+      <c r="G152" s="37" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A153" s="47"/>
+      <c r="B153" s="47"/>
+      <c r="C153" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D153" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="E153" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="F153" s="20">
+        <v>0.28571428571428598</v>
+      </c>
+      <c r="G153" s="36" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A154" s="47"/>
+      <c r="B154" s="47"/>
+      <c r="C154" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D154" s="27"/>
+      <c r="E154" s="27"/>
+      <c r="F154" s="27">
+        <v>0.67857142857142905</v>
+      </c>
+      <c r="G154" s="37" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A155" s="47"/>
+      <c r="B155" s="47"/>
+      <c r="C155" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D155" s="20"/>
+      <c r="E155" s="20"/>
+      <c r="F155" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="G155" s="43" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A156" s="47"/>
+      <c r="B156" s="47"/>
+      <c r="C156" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D156" s="27"/>
+      <c r="E156" s="27"/>
+      <c r="F156" s="27">
+        <v>7.1428571428571397E-2</v>
+      </c>
+      <c r="G156" s="37" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A157" s="47"/>
+      <c r="B157" s="47"/>
+      <c r="C157" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D157" s="20"/>
+      <c r="E157" s="20"/>
+      <c r="F157" s="20">
+        <v>7.1428571428571397E-2</v>
+      </c>
+      <c r="G157" s="37" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A158" s="47"/>
+      <c r="B158" s="47"/>
+      <c r="C158" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D158" s="27"/>
+      <c r="E158" s="27"/>
+      <c r="F158" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="G158" s="37" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A159" s="47"/>
+      <c r="B159" s="47"/>
+      <c r="C159" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D159" s="20"/>
+      <c r="E159" s="20"/>
+      <c r="F159" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="G159" s="37" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A160" s="47"/>
+      <c r="B160" s="47"/>
+      <c r="C160" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="D160" s="27"/>
+      <c r="E160" s="27"/>
+      <c r="F160" s="27">
+        <v>7.1428571428571397E-2</v>
+      </c>
+      <c r="G160" s="37" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A161" s="47"/>
+      <c r="B161" s="47"/>
+      <c r="C161" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D161" s="20"/>
+      <c r="E161" s="20">
+        <v>0.19354838709677399</v>
+      </c>
+      <c r="F161" s="20"/>
+      <c r="G161" s="36"/>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A162" s="47"/>
+      <c r="B162" s="47"/>
+      <c r="C162" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D162" s="27"/>
+      <c r="E162" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="F162" s="27"/>
+      <c r="G162" s="37"/>
+    </row>
+    <row r="163" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A163" s="48"/>
+      <c r="B163" s="48"/>
+      <c r="C163" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D163" s="29"/>
+      <c r="E163" s="29">
+        <v>6.4516129032258104E-2</v>
+      </c>
+      <c r="F163" s="29"/>
+      <c r="G163" s="39"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="A114:A163"/>
+    <mergeCell ref="B115:B124"/>
+    <mergeCell ref="B125:B163"/>
+    <mergeCell ref="A2:A51"/>
+    <mergeCell ref="B2:B11"/>
+    <mergeCell ref="B12:B51"/>
+    <mergeCell ref="A54:A111"/>
+    <mergeCell ref="B55:B64"/>
+    <mergeCell ref="B65:B111"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -4627,7 +7524,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100483727557648AA40B029C215891F95C5" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d36f379eec1cf084072dcf956aecbcf8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8c008993-a31f-4b40-b1f3-88dd9c6e1924" xmlns:ns4="360018dd-41eb-4458-b1d4-4b46a95a2b02" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bd1f472f1ef3281fe4dbeb8213942d38" ns3:_="" ns4:_="">
     <xsd:import namespace="8c008993-a31f-4b40-b1f3-88dd9c6e1924"/>
@@ -4856,24 +7753,13 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57CCF544-D6E5-42F6-A35F-3D4F2EBA47AD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="360018dd-41eb-4458-b1d4-4b46a95a2b02"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="8c008993-a31f-4b40-b1f3-88dd9c6e1924"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{202A38C9-2EAB-4F2A-83A0-C7DD5A2DA12E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -4881,7 +7767,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11C6C962-298D-442F-913D-3477D7E61B99}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4898,4 +7784,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57CCF544-D6E5-42F6-A35F-3D4F2EBA47AD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="360018dd-41eb-4458-b1d4-4b46a95a2b02"/>
+    <ds:schemaRef ds:uri="8c008993-a31f-4b40-b1f3-88dd9c6e1924"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>